<commit_message>
Primera versión del proyecto
</commit_message>
<xml_diff>
--- a/Insumos/insumos_adicionales/data Megatiendas.xlsx
+++ b/Insumos/insumos_adicionales/data Megatiendas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://xpertgroup1-my.sharepoint.com/personal/daniel_jaramillo_xpertgroup_co/Documents/Daniel - Staffing CN/Proyectos Comercial Nutresa/PDFS_Facturas/Insumos/insumos_adicionales/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{29756A16-5165-4EFF-B1C3-03ACC61848F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F78A34E9-0003-4C19-B7BC-ED3263B7D21C}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{29756A16-5165-4EFF-B1C3-03ACC61848F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2612A688-8CFF-40CF-9A63-AC3749E1194D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -359,13 +359,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,7 +652,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -673,7 +676,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
+      <c r="A2" s="6">
         <v>10283523</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -687,7 +690,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="A3" s="6">
         <v>10409942</v>
       </c>
       <c r="B3" s="4" t="s">

</xml_diff>